<commit_message>
Research files for device values
</commit_message>
<xml_diff>
--- a/misc/consumption_types/Groepadressen ETS.xlsx
+++ b/misc/consumption_types/Groepadressen ETS.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihdan\stack\Selficient\databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihdan\git\Home\misc\consumption_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BD22C3-62D7-40C3-85F4-EB0C63CD3D95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25954E6-6BD9-4802-85EF-9FCC0CB2E602}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" xr2:uid="{B2796A8A-9624-47BC-8DDB-495862648000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{B2796A8A-9624-47BC-8DDB-495862648000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
-    <sheet name="Datatypes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="342">
   <si>
     <t>Badkamer spots</t>
   </si>
@@ -1018,36 +1017,9 @@
     <t>**EM = energy module</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>1 bit(boolean)</t>
-  </si>
-  <si>
-    <t>4  bits(3 bit evaluated)</t>
-  </si>
-  <si>
-    <t>1 byte usigned integer</t>
-  </si>
-  <si>
-    <t>2 byte floating point</t>
-  </si>
-  <si>
-    <t>3 byte unsigned integer</t>
-  </si>
-  <si>
-    <t>14 byte ASCII</t>
-  </si>
-  <si>
     <t>Data_type(ID)</t>
   </si>
   <si>
-    <t>1,1,3,5,5</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -1057,25 +1029,28 @@
     <t>1 = heating</t>
   </si>
   <si>
-    <t>9,5,9,-</t>
-  </si>
-  <si>
     <t>NIET STUREN GAAT VIA 2/1/0</t>
   </si>
   <si>
-    <t>1,1,5,5</t>
-  </si>
-  <si>
     <t>1 = auto</t>
   </si>
   <si>
-    <t>1,5,5,5,9</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>Not important</t>
+  </si>
+  <si>
+    <t>1,1,15,2,2</t>
+  </si>
+  <si>
+    <t>1,1,2,2</t>
+  </si>
+  <si>
+    <t>4,2,4,-</t>
+  </si>
+  <si>
+    <t>1,2,2,2,4</t>
   </si>
 </sst>
 </file>
@@ -1146,13 +1121,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1469,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB25D090-3CF4-4764-BEB6-299A255129C0}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,15 +1463,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1514,10 +1491,10 @@
         <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,7 +1517,7 @@
         <v>27</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,8 +1539,8 @@
       <c r="F4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>339</v>
+      <c r="G4" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1585,8 +1562,8 @@
       <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>339</v>
+      <c r="G5" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1608,8 +1585,8 @@
       <c r="F6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>339</v>
+      <c r="G6" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1631,8 +1608,8 @@
       <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>339</v>
+      <c r="G7" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1654,8 +1631,8 @@
       <c r="F8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>339</v>
+      <c r="G8" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1677,8 +1654,8 @@
       <c r="F9" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>339</v>
+      <c r="G9" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1700,8 +1677,8 @@
       <c r="F10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>339</v>
+      <c r="G10" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,19 +1700,19 @@
       <c r="F11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>339</v>
+      <c r="G11" s="7" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1743,10 +1720,10 @@
         <v>278</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1758,24 +1735,24 @@
         <v>279</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1791,10 +1768,10 @@
         <v>147</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1811,7 +1788,7 @@
         <v>141</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1827,8 +1804,8 @@
       <c r="D20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>343</v>
+      <c r="F20" s="7" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1844,8 +1821,8 @@
       <c r="D21" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>343</v>
+      <c r="F21" s="7" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1856,22 +1833,22 @@
         <v>149</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -1891,10 +1868,10 @@
         <v>49</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1914,7 +1891,7 @@
         <v>275</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1933,8 +1910,8 @@
       <c r="E27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>345</v>
+      <c r="G27" s="7" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1953,8 +1930,8 @@
       <c r="E28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>345</v>
+      <c r="G28" s="7" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1973,8 +1950,8 @@
       <c r="E29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>345</v>
+      <c r="G29" s="7" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1993,8 +1970,8 @@
       <c r="E30" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>345</v>
+      <c r="G30" s="7" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2013,8 +1990,8 @@
       <c r="E31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>345</v>
+      <c r="G31" s="7" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2025,7 +2002,7 @@
         <v>95</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2036,7 +2013,7 @@
         <v>96</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2047,7 +2024,7 @@
         <v>97</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2058,7 +2035,7 @@
         <v>98</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2069,21 +2046,21 @@
         <v>99</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
@@ -2105,10 +2082,10 @@
         <v>66</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2134,7 +2111,7 @@
         <v>100</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2159,8 +2136,8 @@
       <c r="G41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>347</v>
+      <c r="H41" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2185,19 +2162,19 @@
       <c r="G42" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>347</v>
+      <c r="H42" s="7" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2207,10 +2184,10 @@
         <v>62</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="F45" s="2"/>
     </row>
@@ -2225,10 +2202,10 @@
         <v>245</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2242,10 +2219,10 @@
         <v>246</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2259,10 +2236,10 @@
         <v>247</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -2276,10 +2253,10 @@
         <v>248</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2293,21 +2270,21 @@
         <v>249</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -2341,10 +2318,10 @@
         <v>238</v>
       </c>
       <c r="L54" s="3" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -2382,10 +2359,10 @@
         <v>254</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -2423,10 +2400,10 @@
         <v>270</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -2464,10 +2441,10 @@
         <v>272</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -2505,10 +2482,10 @@
         <v>273</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -2546,21 +2523,21 @@
         <v>274</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
@@ -2707,14 +2684,14 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="8"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
@@ -2776,14 +2753,14 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
@@ -2986,16 +2963,16 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="10">
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A84:F84"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A84:F84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -3003,80 +2980,4 @@
     <ignoredError sqref="C27:C31 D26:D31" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4DF65F6-D6EB-4AE3-9E25-AAD455FE5523}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>332</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>333</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>334</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>336</v>
-      </c>
-      <c r="B6">
-        <v>232600</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>337</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added 109 devices to database build
</commit_message>
<xml_diff>
--- a/misc/consumption_types/Groepadressen ETS.xlsx
+++ b/misc/consumption_types/Groepadressen ETS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihdan\git\Home\misc\consumption_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25954E6-6BD9-4802-85EF-9FCC0CB2E602}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D5FC0B-3A01-4922-BBF9-DCB0EBA483DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{B2796A8A-9624-47BC-8DDB-495862648000}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12360" xr2:uid="{B2796A8A-9624-47BC-8DDB-495862648000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="344">
   <si>
     <t>Badkamer spots</t>
   </si>
@@ -1051,13 +1051,19 @@
   </si>
   <si>
     <t>1,2,2,2,4</t>
+  </si>
+  <si>
+    <t>Hoeft nog niet</t>
+  </si>
+  <si>
+    <t>AANPASSEN!!!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1080,13 +1086,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1098,10 +1116,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1124,14 +1143,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1446,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB25D090-3CF4-4764-BEB6-299A255129C0}">
   <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,15 +1489,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1705,14 +1731,14 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1740,19 +1766,22 @@
       <c r="E15" s="1" t="s">
         <v>333</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
@@ -1841,14 +1870,14 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
@@ -2053,14 +2082,14 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
@@ -2167,14 +2196,14 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2277,14 +2306,17 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
+      <c r="A53" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="1" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
@@ -2530,14 +2562,14 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
+      <c r="A61" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
@@ -2684,17 +2716,17 @@
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="8" t="s">
         <v>230</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -2753,17 +2785,17 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
+      <c r="A84" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="8" t="s">
         <v>284</v>
       </c>
       <c r="F85" s="2"/>
@@ -2821,7 +2853,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="8" t="s">
         <v>285</v>
       </c>
     </row>
@@ -2882,7 +2914,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="8" t="s">
         <v>287</v>
       </c>
     </row>
@@ -2940,7 +2972,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="8" t="s">
         <v>320</v>
       </c>
     </row>
@@ -2963,16 +2995,16 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="10">
-    <mergeCell ref="A78:F78"/>
-    <mergeCell ref="A44:F44"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A61:F61"/>
     <mergeCell ref="A84:F84"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A53:F53"/>
     <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A78:F78"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A61:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>